<commit_message>
HP: ExcelToStringArray extended with writeToCell method
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/test.xlsx
+++ b/SerialXmlZipProcessor/data/excel/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
   <si>
     <t>test</t>
   </si>
@@ -70,12 +70,16 @@
   </si>
   <si>
     <t>item11</t>
+  </si>
+  <si>
+    <t>NEW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +462,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>